<commit_message>
Modified keyword " open tHe session" and Running test suites parallel on different browser
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/add_to_cart_test_data.xlsx
+++ b/TestData/Web_POS/Billing/add_to_cart_test_data.xlsx
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>usertwo_p1</t>
+  </si>
+  <si>
+    <t>2000 : 1</t>
+  </si>
+  <si>
+    <t>500 : 1</t>
   </si>
   <si>
     <t>Index9QA</t>
@@ -469,8 +475,8 @@
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="I1">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -572,37 +578,37 @@
       <c r="F2" s="2">
         <v>123456</v>
       </c>
-      <c r="G2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>500</v>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L2" s="3">
         <v>45384</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -626,30 +632,30 @@
         <v>500</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L3" s="3">
         <v>45384</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" ht="31.5" customHeight="1">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
@@ -673,30 +679,30 @@
         <v>300</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L4" s="3">
         <v>45384</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -720,33 +726,33 @@
         <v>400</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L5" s="3">
         <v>45384</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" ht="26.25" customHeight="1">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -755,7 +761,7 @@
         <v>123456</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2">
         <v>123456</v>
@@ -767,30 +773,30 @@
         <v>800</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L6" s="3">
         <v>45384</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>17</v>
@@ -814,33 +820,33 @@
         <v>600</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L7" s="3">
         <v>45384</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" ht="31.5" customHeight="1">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
@@ -849,7 +855,7 @@
         <v>123456</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2">
         <v>123456</v>
@@ -861,30 +867,30 @@
         <v>600</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L8" s="3">
         <v>45384</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" ht="32.25" customHeight="1">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -908,33 +914,33 @@
         <v>600</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L9" s="3">
         <v>45384</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" ht="28.5" customHeight="1">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
@@ -943,7 +949,7 @@
         <v>123456</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F10" s="2">
         <v>123456</v>
@@ -955,30 +961,30 @@
         <v>600</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L10" s="3">
         <v>45384</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
@@ -1002,30 +1008,30 @@
         <v>600</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L11" s="3">
         <v>45384</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -1049,30 +1055,30 @@
         <v>600</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L12" s="3">
         <v>45384</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1096,33 +1102,33 @@
         <v>600</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L13" s="3">
         <v>45384</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -1131,7 +1137,7 @@
         <v>123456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2">
         <v>123456</v>
@@ -1143,30 +1149,30 @@
         <v>600</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L14" s="3">
         <v>45384</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -1190,33 +1196,33 @@
         <v>600</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L15" s="3">
         <v>45384</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -1225,7 +1231,7 @@
         <v>123456</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F16" s="2">
         <v>123456</v>
@@ -1237,30 +1243,30 @@
         <v>600</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L16" s="3">
         <v>45384</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -1284,30 +1290,30 @@
         <v>600</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L17" s="3">
         <v>45384</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1331,30 +1337,30 @@
         <v>600</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L18" s="3">
         <v>45384</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>17</v>
@@ -1378,25 +1384,25 @@
         <v>600</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L19" s="3">
         <v>45384</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" ht="14.25">
@@ -1560,7 +1566,7 @@
       <c r="F38" s="2"/>
       <c r="I38" s="1"/>
       <c r="K38" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -1579,7 +1585,7 @@
       <c r="F39" s="2"/>
       <c r="I39" s="1"/>
       <c r="K39" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -1594,7 +1600,7 @@
       <c r="F40" s="2"/>
       <c r="I40" s="1"/>
       <c r="K40" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -1609,7 +1615,7 @@
       <c r="F41" s="2"/>
       <c r="I41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -1624,7 +1630,7 @@
       <c r="F42" s="2"/>
       <c r="I42" s="1"/>
       <c r="K42" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -1639,7 +1645,7 @@
       <c r="F43" s="2"/>
       <c r="I43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
@@ -1654,7 +1660,7 @@
       <c r="F44" s="2"/>
       <c r="I44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
@@ -1669,7 +1675,7 @@
       <c r="F45" s="2"/>
       <c r="I45" s="1"/>
       <c r="K45" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
@@ -1684,7 +1690,7 @@
       <c r="F46" s="2"/>
       <c r="I46" s="1"/>
       <c r="K46" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -1699,7 +1705,7 @@
       <c r="F47" s="2"/>
       <c r="I47" s="1"/>
       <c r="K47" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>

</xml_diff>

<commit_message>
Closing and opening balance change
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/add_to_cart_test_data.xlsx
+++ b/TestData/Web_POS/Billing/add_to_cart_test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\Web_POS\Billing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Indexnine\PycharmProjects\zwing-qa-automation\TestData\Web_POS\Billing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>usertwo_p1</t>
+  </si>
+  <si>
+    <t>2000 : 1</t>
+  </si>
+  <si>
+    <t>500 : 1</t>
   </si>
   <si>
     <t>Index9QA</t>
@@ -469,8 +475,8 @@
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="I1">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A5">
+      <selection activeCell="G2" sqref="G2:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -572,37 +578,37 @@
       <c r="F2" s="2">
         <v>123456</v>
       </c>
-      <c r="G2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H2" s="1">
-        <v>500</v>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L2" s="3">
         <v>45384</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -619,37 +625,37 @@
       <c r="F3" s="2">
         <v>123456</v>
       </c>
-      <c r="G3">
-        <v>1000</v>
-      </c>
-      <c r="H3">
-        <v>500</v>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L3" s="3">
         <v>45384</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" ht="31.5" customHeight="1">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
@@ -666,37 +672,37 @@
       <c r="F4" s="2">
         <v>123456</v>
       </c>
-      <c r="G4">
-        <v>1000</v>
-      </c>
-      <c r="H4">
-        <v>300</v>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L4" s="3">
         <v>45384</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
@@ -713,40 +719,40 @@
       <c r="F5" s="2">
         <v>123456</v>
       </c>
-      <c r="G5">
-        <v>1000</v>
-      </c>
-      <c r="H5">
-        <v>400</v>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L5" s="3">
         <v>45384</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" ht="26.25" customHeight="1">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -755,42 +761,42 @@
         <v>123456</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2">
         <v>123456</v>
       </c>
-      <c r="G6">
-        <v>1000</v>
-      </c>
-      <c r="H6">
-        <v>800</v>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L6" s="3">
         <v>45384</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>17</v>
@@ -807,40 +813,40 @@
       <c r="F7" s="2">
         <v>123456</v>
       </c>
-      <c r="G7">
-        <v>1000</v>
-      </c>
-      <c r="H7">
-        <v>600</v>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L7" s="3">
         <v>45384</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" ht="31.5" customHeight="1">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>18</v>
@@ -849,42 +855,42 @@
         <v>123456</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2">
         <v>123456</v>
       </c>
-      <c r="G8">
-        <v>1000</v>
-      </c>
-      <c r="H8">
-        <v>600</v>
+      <c r="G8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L8" s="3">
         <v>45384</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" ht="32.25" customHeight="1">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
@@ -901,40 +907,40 @@
       <c r="F9" s="2">
         <v>123456</v>
       </c>
-      <c r="G9">
-        <v>1000</v>
-      </c>
-      <c r="H9">
-        <v>600</v>
+      <c r="G9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L9" s="3">
         <v>45384</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" ht="28.5" customHeight="1">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>18</v>
@@ -943,42 +949,42 @@
         <v>123456</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F10" s="2">
         <v>123456</v>
       </c>
-      <c r="G10">
-        <v>1000</v>
-      </c>
-      <c r="H10">
-        <v>600</v>
+      <c r="G10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L10" s="3">
         <v>45384</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>17</v>
@@ -995,37 +1001,37 @@
       <c r="F11" s="2">
         <v>123456</v>
       </c>
-      <c r="G11">
-        <v>1000</v>
-      </c>
-      <c r="H11">
-        <v>600</v>
+      <c r="G11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L11" s="3">
         <v>45384</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>17</v>
@@ -1042,37 +1048,37 @@
       <c r="F12" s="2">
         <v>123456</v>
       </c>
-      <c r="G12">
-        <v>1000</v>
-      </c>
-      <c r="H12">
-        <v>600</v>
+      <c r="G12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L12" s="3">
         <v>45384</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1089,40 +1095,40 @@
       <c r="F13" s="2">
         <v>123456</v>
       </c>
-      <c r="G13">
-        <v>1000</v>
-      </c>
-      <c r="H13">
-        <v>600</v>
+      <c r="G13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L13" s="3">
         <v>45384</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>18</v>
@@ -1131,42 +1137,42 @@
         <v>123456</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2">
         <v>123456</v>
       </c>
-      <c r="G14">
-        <v>1000</v>
-      </c>
-      <c r="H14">
-        <v>600</v>
+      <c r="G14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L14" s="3">
         <v>45384</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
@@ -1183,40 +1189,40 @@
       <c r="F15" s="2">
         <v>123456</v>
       </c>
-      <c r="G15">
-        <v>1000</v>
-      </c>
-      <c r="H15">
-        <v>600</v>
+      <c r="G15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L15" s="3">
         <v>45384</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -1225,42 +1231,42 @@
         <v>123456</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F16" s="2">
         <v>123456</v>
       </c>
-      <c r="G16">
-        <v>1000</v>
-      </c>
-      <c r="H16">
-        <v>600</v>
+      <c r="G16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L16" s="3">
         <v>45384</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
@@ -1277,37 +1283,37 @@
       <c r="F17" s="2">
         <v>123456</v>
       </c>
-      <c r="G17">
-        <v>1000</v>
-      </c>
-      <c r="H17">
-        <v>600</v>
+      <c r="G17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L17" s="3">
         <v>45384</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -1324,37 +1330,37 @@
       <c r="F18" s="2">
         <v>123456</v>
       </c>
-      <c r="G18">
-        <v>1000</v>
-      </c>
-      <c r="H18">
-        <v>600</v>
+      <c r="G18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L18" s="3">
         <v>45384</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>17</v>
@@ -1371,32 +1377,32 @@
       <c r="F19" s="2">
         <v>123456</v>
       </c>
-      <c r="G19">
-        <v>1000</v>
-      </c>
-      <c r="H19">
-        <v>600</v>
+      <c r="G19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L19" s="3">
         <v>45384</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" ht="14.25">
@@ -1560,7 +1566,7 @@
       <c r="F38" s="2"/>
       <c r="I38" s="1"/>
       <c r="K38" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -1579,7 +1585,7 @@
       <c r="F39" s="2"/>
       <c r="I39" s="1"/>
       <c r="K39" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -1594,7 +1600,7 @@
       <c r="F40" s="2"/>
       <c r="I40" s="1"/>
       <c r="K40" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -1609,7 +1615,7 @@
       <c r="F41" s="2"/>
       <c r="I41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -1624,7 +1630,7 @@
       <c r="F42" s="2"/>
       <c r="I42" s="1"/>
       <c r="K42" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -1639,7 +1645,7 @@
       <c r="F43" s="2"/>
       <c r="I43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
@@ -1654,7 +1660,7 @@
       <c r="F44" s="2"/>
       <c r="I44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
@@ -1669,7 +1675,7 @@
       <c r="F45" s="2"/>
       <c r="I45" s="1"/>
       <c r="K45" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
@@ -1684,7 +1690,7 @@
       <c r="F46" s="2"/>
       <c r="I46" s="1"/>
       <c r="K46" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -1699,7 +1705,7 @@
       <c r="F47" s="2"/>
       <c r="I47" s="1"/>
       <c r="K47" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>

</xml_diff>